<commit_message>
Refactoring the web app. Splitting the css and js into seperate files to make things more readable. Formalizing the widget behaviors and documenting in a md file.
</commit_message>
<xml_diff>
--- a/UI_Webpage/layout plan.xlsx
+++ b/UI_Webpage/layout plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://labtestcertificationinc-my.sharepoint.com/personal/kdhillon_labtestcert_com/Documents/LabTestCert/LC Test Streams/S0900 - Fenestration Wall Testing/A. Test Apparatus/D. Toronto Fenestration Wall/A. Components/C0 - Controller/.A - Software/UI_Webpage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BECB2014-8E6D-4B2B-AFA4-3F29705D6105}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610F7BC4-C756-4B23-8AB1-A2715E995889}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>text)</a:t>
+            <a:t>label-value)</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
@@ -588,11 +588,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" b="1"/>
-            <a:t>(Short </a:t>
+            <a:t>(label-value</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>text)</a:t>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
@@ -888,11 +888,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" b="1"/>
-            <a:t>(live </a:t>
+            <a:t>(smart-label-value</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>text)</a:t>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
@@ -1660,7 +1660,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Lots happened. Updated OSBos so that it now accepts terminal tasks with callbacks. Added button widgets. Started adding smart-label-value widgets (not done yet). Updated the web server infrastructure so that it can work with async terminal tasks from OSBos, so now the WebApp can initiate a long-running task, and the server will work away at the task asynchronously, and then respond back to the client when the task finishes. This was hard. There is now an example where the user can click the example button on the web app, then the server will turn the CPU light blue for 2 seconds, then turn it back to green and respond to the client with a success message.
</commit_message>
<xml_diff>
--- a/UI_Webpage/layout plan.xlsx
+++ b/UI_Webpage/layout plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://labtestcertificationinc-my.sharepoint.com/personal/kdhillon_labtestcert_com/Documents/LabTestCert/LC Test Streams/S0900 - Fenestration Wall Testing/A. Test Apparatus/D. Toronto Fenestration Wall/A. Components/C0 - Controller/.A - Software/UI_Webpage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610F7BC4-C756-4B23-8AB1-A2715E995889}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156CF461-EDFB-4408-9ADE-0F322FD1CF1C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
   </bookViews>
@@ -485,18 +485,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent6"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -560,18 +558,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent6"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>

</xml_diff>

<commit_message>
no idea what changed since last time. sue me.
</commit_message>
<xml_diff>
--- a/UI_Webpage/layout plan.xlsx
+++ b/UI_Webpage/layout plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://labtestcertificationinc-my.sharepoint.com/personal/kdhillon_labtestcert_com/Documents/LabTestCert/LC Test Streams/S0900 - Fenestration Wall Testing/A. Test Apparatus/D. Toronto Fenestration Wall/A. Components/C0 - Controller/.A - Software/UI_Webpage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156CF461-EDFB-4408-9ADE-0F322FD1CF1C}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B60B40D-893D-4E27-8C5A-0FB2E2B1456A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,15 +90,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -113,7 +113,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2381250" y="2476500"/>
+          <a:off x="2352675" y="3314700"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -122,18 +122,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -165,15 +163,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -188,7 +186,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4552950" y="2476500"/>
+          <a:off x="4524375" y="3314700"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -197,18 +195,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -240,15 +236,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -263,7 +259,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="5095875"/>
+          <a:off x="2343150" y="5934075"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -272,18 +268,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -315,15 +309,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -338,7 +332,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4552950" y="5095875"/>
+          <a:off x="4524375" y="5934075"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -347,18 +341,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -390,15 +382,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -413,7 +405,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="3133725"/>
+          <a:off x="2343150" y="3971925"/>
           <a:ext cx="4295775" cy="1866900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -453,15 +445,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -476,7 +468,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="590550"/>
+          <a:off x="2343150" y="1428750"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -526,15 +518,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -549,7 +541,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4543425" y="581025"/>
+          <a:off x="4514850" y="1419225"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -599,15 +591,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -622,7 +614,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4552950" y="1228725"/>
+          <a:off x="4524375" y="2066925"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -631,18 +623,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -674,15 +664,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -697,7 +687,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="1857375"/>
+          <a:off x="2333625" y="2695575"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -706,18 +696,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -749,15 +737,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -772,7 +760,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4562475" y="1857375"/>
+          <a:off x="4533900" y="2695575"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -781,18 +769,16 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -824,15 +810,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -847,7 +833,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="1238250"/>
+          <a:off x="2333625" y="2076450"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -856,15 +842,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="accent6">
             <a:shade val="15000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent6"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent6"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -1326,6 +1312,152 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
             <a:t> text)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FE6826-AB5B-487E-B9CF-C03BB207053F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2343150" y="800100"/>
+          <a:ext cx="2105025" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>STOP_ALL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>(button</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rectangle 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA0DCD1-2963-4AE3-330E-DDAF530A70FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4514850" y="800100"/>
+          <a:ext cx="2105025" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>targetPressure</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1"/>
+            <a:t>(value-sender</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
@@ -1656,7 +1788,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hooked up analog inputs in the HAL. Connected some HAL endpoints to the UI through the WebServer. Updated digital outputs on the HAL. The hardware I/O is nicely abstracted now. Did I have the MechanicalSystem.h set up in the last commit? Well that's there now. Business logic threads and tasks for the mechanical system.
</commit_message>
<xml_diff>
--- a/UI_Webpage/layout plan.xlsx
+++ b/UI_Webpage/layout plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://labtestcertificationinc-my.sharepoint.com/personal/kdhillon_labtestcert_com/Documents/LabTestCert/LC Test Streams/S0900 - Fenestration Wall Testing/A. Test Apparatus/D. Toronto Fenestration Wall/A. Components/C0 - Controller/.A - Software/UI_Webpage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B60B40D-893D-4E27-8C5A-0FB2E2B1456A}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EE6941C-8D24-4E32-AC4A-8BA18DB347B6}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
   </bookViews>
@@ -623,16 +623,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -696,16 +698,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -769,16 +773,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -842,15 +848,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6">
+          <a:schemeClr val="accent3">
             <a:shade val="15000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent3"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -1354,16 +1360,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -1427,16 +1435,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>

</xml_diff>

<commit_message>
Added functions to examine the RAM and determine how much of it we are using/how much is free. Connected the logger to the HAL. Set up logging once per second. Connected the logger to the WebApp. Checks to make sure the memory is safe with all features running.
</commit_message>
<xml_diff>
--- a/UI_Webpage/layout plan.xlsx
+++ b/UI_Webpage/layout plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://labtestcertificationinc-my.sharepoint.com/personal/kdhillon_labtestcert_com/Documents/LabTestCert/LC Test Streams/S0900 - Fenestration Wall Testing/A. Test Apparatus/D. Toronto Fenestration Wall/A. Components/C0 - Controller/.A - Software/UI_Webpage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EE6941C-8D24-4E32-AC4A-8BA18DB347B6}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{CC2BBCA5-8B71-4EF3-8875-D7EAA5356268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FB51A3-486E-4943-BE12-D423A11DDD52}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71A5893A-0805-420F-8C5E-EDEF138E9C36}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,16 +123,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -195,16 +198,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -268,16 +273,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -341,16 +348,18 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -815,16 +824,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -839,7 +848,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2333625" y="2076450"/>
+          <a:off x="4514850" y="790575"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1402,16 +1411,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1426,7 +1435,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4514850" y="800100"/>
+          <a:off x="2343150" y="2047875"/>
           <a:ext cx="2105025" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1476,6 +1485,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1798,7 +1811,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>